<commit_message>
process of working with yolo, cant understand and model is not doing its job, cant crop properly
</commit_message>
<xml_diff>
--- a/Train_Yolo_Coordinates.xlsx
+++ b/Train_Yolo_Coordinates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario 1\Desktop\DarioInfo\OJIAR\sistema_agentes_img_ojiar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB98836-FEBA-46AD-8074-8340BD8825BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7396D9A1-9663-49F8-B176-392B61D31AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7AB2FE51-A8F8-410B-A035-2A0E495249CF}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <dimension ref="B1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
trained yolo to make better crops
</commit_message>
<xml_diff>
--- a/Train_Yolo_Coordinates.xlsx
+++ b/Train_Yolo_Coordinates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario 1\Desktop\DarioInfo\OJIAR\sistema_agentes_img_ojiar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7396D9A1-9663-49F8-B176-392B61D31AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE29656D-8D2B-4A2A-B475-9078A5954A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7AB2FE51-A8F8-410B-A035-2A0E495249CF}"/>
   </bookViews>
@@ -67,7 +67,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,16 +106,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,12 +440,13 @@
   <dimension ref="B1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="4" width="11.08984375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.35">
@@ -438,37 +461,37 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>4821</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="4">
+        <v>4961</v>
+      </c>
+      <c r="D2" s="4">
         <v>4016</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1">
-        <v>132</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1928</v>
+      <c r="C4" s="4">
+        <v>185</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2205</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
-        <v>1215</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2757</v>
+      <c r="C5" s="4">
+        <v>1025</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2754</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
@@ -479,41 +502,41 @@
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <f>(C4+C5)/2/C2</f>
-        <v>0.13970130678282514</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>0.12195121951219512</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <f>(D4+D5)/2/D2</f>
-        <v>0.58329183266932272</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>0.61740537848605581</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <f>(C5-C4)/C2</f>
-        <v>0.22464219041692596</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>0.16932070147147751</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <f>(D5-D4)/D2</f>
-        <v>0.20642430278884463</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>0.13670318725099601</v>
+      </c>
+      <c r="D10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>